<commit_message>
Modul 7 - Databaser
</commit_message>
<xml_diff>
--- a/Modul 7 - Databaser/videobutik/videobutik.xlsx
+++ b/Modul 7 - Databaser/videobutik/videobutik.xlsx
@@ -5,23 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\webbprogrammering\Modul 7 - Databaser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\webbprogrammering\Modul 7 - Databaser\videobutik\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="43" windowWidth="11357" windowHeight="8443" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="43" windowWidth="11357" windowHeight="8443" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kund" sheetId="3" r:id="rId1"/>
     <sheet name="Film" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId3"/>
+    <sheet name="Uthyrning" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="367">
   <si>
     <t>Matrix</t>
   </si>
@@ -1110,9 +1110,6 @@
   </si>
   <si>
     <t>Django Reinhardt</t>
-  </si>
-  <si>
-    <t>Kundnummer</t>
   </si>
   <si>
     <t>Film</t>
@@ -1454,1728 +1451,1428 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.3046875" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.61328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>363</v>
+        <v>159</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>159</v>
+        <v>258</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="E1" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>11356</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>11356</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>12567</v>
+      </c>
+      <c r="D3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>12578</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>15336</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>16537</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>268</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>15467</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>269</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>71434</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>270</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>68433</v>
+      </c>
+      <c r="D9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>264</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>12567</v>
-      </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>271</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>15666</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>272</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>25678</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>273</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>65833</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>274</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13">
+        <v>15784</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>275</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>77456</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>276</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15">
+        <v>25467</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>277</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>84624</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>278</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <v>99965</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>279</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18">
+        <v>15489</v>
+      </c>
+      <c r="D18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>265</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>12578</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>280</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19">
+        <v>14354</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>281</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20">
+        <v>42367</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>282</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21">
+        <v>37689</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>283</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22">
+        <v>25478</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>284</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23">
+        <v>15478</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>285</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24">
+        <v>73447</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>286</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25">
+        <v>26589</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>287</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26">
+        <v>15894</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>288</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27">
+        <v>26478</v>
+      </c>
+      <c r="D27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>289</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28">
+        <v>55567</v>
+      </c>
+      <c r="D28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>290</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29">
+        <v>35467</v>
+      </c>
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>291</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30">
+        <v>25489</v>
+      </c>
+      <c r="D30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>292</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31">
+        <v>12356</v>
+      </c>
+      <c r="D31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>293</v>
+      </c>
+      <c r="B32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32">
+        <v>97834</v>
+      </c>
+      <c r="D32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>294</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33">
+        <v>85678</v>
+      </c>
+      <c r="D33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>295</v>
+      </c>
+      <c r="B34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34">
+        <v>72356</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>296</v>
+      </c>
+      <c r="B35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35">
+        <v>68745</v>
+      </c>
+      <c r="D35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>297</v>
+      </c>
+      <c r="B36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36">
+        <v>57789</v>
+      </c>
+      <c r="D36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>298</v>
+      </c>
+      <c r="B37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37">
+        <v>46576</v>
+      </c>
+      <c r="D37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>299</v>
+      </c>
+      <c r="B38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38">
+        <v>34598</v>
+      </c>
+      <c r="D38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>300</v>
+      </c>
+      <c r="B39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39">
+        <v>24444</v>
+      </c>
+      <c r="D39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>301</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40">
+        <v>15368</v>
+      </c>
+      <c r="D40" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>266</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>15336</v>
-      </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>302</v>
+      </c>
+      <c r="B41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41">
+        <v>17689</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>303</v>
+      </c>
+      <c r="B42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42">
+        <v>15456</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>304</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43">
+        <v>16278</v>
+      </c>
+      <c r="D43" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>305</v>
+      </c>
+      <c r="B44" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44">
+        <v>11111</v>
+      </c>
+      <c r="D44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>306</v>
+      </c>
+      <c r="B45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45">
+        <v>54634</v>
+      </c>
+      <c r="D45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>307</v>
+      </c>
+      <c r="B46" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46">
+        <v>15489</v>
+      </c>
+      <c r="D46" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>308</v>
+      </c>
+      <c r="B47" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47">
+        <v>67677</v>
+      </c>
+      <c r="D47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>309</v>
+      </c>
+      <c r="B48" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48">
+        <v>24356</v>
+      </c>
+      <c r="D48" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>310</v>
+      </c>
+      <c r="B49" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49">
+        <v>36567</v>
+      </c>
+      <c r="D49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>311</v>
+      </c>
+      <c r="B50" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50">
+        <v>79834</v>
+      </c>
+      <c r="D50" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>312</v>
+      </c>
+      <c r="B51" t="s">
+        <v>79</v>
+      </c>
+      <c r="C51">
+        <v>26567</v>
+      </c>
+      <c r="D51" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>313</v>
+      </c>
+      <c r="B52" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52">
+        <v>14356</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>314</v>
+      </c>
+      <c r="B53" t="s">
+        <v>81</v>
+      </c>
+      <c r="C53">
+        <v>15378</v>
+      </c>
+      <c r="D53" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>315</v>
+      </c>
+      <c r="B54" t="s">
+        <v>83</v>
+      </c>
+      <c r="C54">
+        <v>25567</v>
+      </c>
+      <c r="D54" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>316</v>
+      </c>
+      <c r="B55" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55">
+        <v>38699</v>
+      </c>
+      <c r="D55" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>317</v>
+      </c>
+      <c r="B56" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56">
+        <v>44444</v>
+      </c>
+      <c r="D56" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>318</v>
+      </c>
+      <c r="B57" t="s">
+        <v>88</v>
+      </c>
+      <c r="C57">
+        <v>52468</v>
+      </c>
+      <c r="D57" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>319</v>
+      </c>
+      <c r="B58" t="s">
+        <v>90</v>
+      </c>
+      <c r="C58">
+        <v>61789</v>
+      </c>
+      <c r="D58" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>320</v>
+      </c>
+      <c r="B59" t="s">
+        <v>92</v>
+      </c>
+      <c r="C59">
+        <v>71508</v>
+      </c>
+      <c r="D59" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>321</v>
+      </c>
+      <c r="B60" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60">
+        <v>82154</v>
+      </c>
+      <c r="D60" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>322</v>
+      </c>
+      <c r="B61" t="s">
+        <v>96</v>
+      </c>
+      <c r="C61">
+        <v>96734</v>
+      </c>
+      <c r="D61" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>323</v>
+      </c>
+      <c r="B62" t="s">
+        <v>98</v>
+      </c>
+      <c r="C62">
+        <v>13254</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>324</v>
+      </c>
+      <c r="B63" t="s">
+        <v>99</v>
+      </c>
+      <c r="C63">
+        <v>17690</v>
+      </c>
+      <c r="D63" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>325</v>
+      </c>
+      <c r="B64" t="s">
+        <v>101</v>
+      </c>
+      <c r="C64">
+        <v>37589</v>
+      </c>
+      <c r="D64" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>326</v>
+      </c>
+      <c r="B65" t="s">
+        <v>103</v>
+      </c>
+      <c r="C65">
+        <v>62587</v>
+      </c>
+      <c r="D65" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>327</v>
+      </c>
+      <c r="B66" t="s">
+        <v>105</v>
+      </c>
+      <c r="C66">
+        <v>58696</v>
+      </c>
+      <c r="D66" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>328</v>
+      </c>
+      <c r="B67" t="s">
+        <v>107</v>
+      </c>
+      <c r="C67">
+        <v>16470</v>
+      </c>
+      <c r="D67" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>329</v>
+      </c>
+      <c r="B68" t="s">
+        <v>109</v>
+      </c>
+      <c r="C68">
+        <v>15367</v>
+      </c>
+      <c r="D68" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>330</v>
+      </c>
+      <c r="B69" t="s">
+        <v>111</v>
+      </c>
+      <c r="C69">
+        <v>72656</v>
+      </c>
+      <c r="D69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>331</v>
+      </c>
+      <c r="B70" t="s">
+        <v>112</v>
+      </c>
+      <c r="C70">
+        <v>28567</v>
+      </c>
+      <c r="D70" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>332</v>
+      </c>
+      <c r="B71" t="s">
+        <v>114</v>
+      </c>
+      <c r="C71">
+        <v>85645</v>
+      </c>
+      <c r="D71" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>333</v>
+      </c>
+      <c r="B72" t="s">
+        <v>116</v>
+      </c>
+      <c r="C72">
+        <v>12134</v>
+      </c>
+      <c r="D72" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>334</v>
+      </c>
+      <c r="B73" t="s">
+        <v>117</v>
+      </c>
+      <c r="C73">
+        <v>18467</v>
+      </c>
+      <c r="D73" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>335</v>
+      </c>
+      <c r="B74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C74">
+        <v>36478</v>
+      </c>
+      <c r="D74" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>336</v>
+      </c>
+      <c r="B75" t="s">
+        <v>120</v>
+      </c>
+      <c r="C75">
+        <v>37788</v>
+      </c>
+      <c r="D75" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>337</v>
+      </c>
+      <c r="B76" t="s">
+        <v>121</v>
+      </c>
+      <c r="C76">
+        <v>31456</v>
+      </c>
+      <c r="D76" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>338</v>
+      </c>
+      <c r="B77" t="s">
+        <v>123</v>
+      </c>
+      <c r="C77">
+        <v>42356</v>
+      </c>
+      <c r="D77" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>339</v>
+      </c>
+      <c r="B78" t="s">
+        <v>125</v>
+      </c>
+      <c r="C78">
+        <v>62599</v>
+      </c>
+      <c r="D78" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>340</v>
+      </c>
+      <c r="B79" t="s">
+        <v>127</v>
+      </c>
+      <c r="C79">
+        <v>25467</v>
+      </c>
+      <c r="D79" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>341</v>
+      </c>
+      <c r="B80" t="s">
+        <v>128</v>
+      </c>
+      <c r="C80">
+        <v>48755</v>
+      </c>
+      <c r="D80" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>342</v>
+      </c>
+      <c r="B81" t="s">
+        <v>130</v>
+      </c>
+      <c r="C81">
+        <v>26478</v>
+      </c>
+      <c r="D81" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>343</v>
+      </c>
+      <c r="B82" t="s">
+        <v>130</v>
+      </c>
+      <c r="C82">
+        <v>26444</v>
+      </c>
+      <c r="D82" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>344</v>
+      </c>
+      <c r="B83" t="s">
+        <v>131</v>
+      </c>
+      <c r="C83">
+        <v>27599</v>
+      </c>
+      <c r="D83" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>345</v>
+      </c>
+      <c r="B84" t="s">
+        <v>132</v>
+      </c>
+      <c r="C84">
+        <v>26476</v>
+      </c>
+      <c r="D84" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>346</v>
+      </c>
+      <c r="B85" t="s">
+        <v>133</v>
+      </c>
+      <c r="C85">
+        <v>11122</v>
+      </c>
+      <c r="D85" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>347</v>
+      </c>
+      <c r="B86" t="s">
+        <v>134</v>
+      </c>
+      <c r="C86">
+        <v>16688</v>
+      </c>
+      <c r="D86" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>348</v>
+      </c>
+      <c r="B87" t="s">
+        <v>135</v>
+      </c>
+      <c r="C87">
+        <v>54678</v>
+      </c>
+      <c r="D87" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>349</v>
+      </c>
+      <c r="B88" t="s">
+        <v>136</v>
+      </c>
+      <c r="C88">
+        <v>55588</v>
+      </c>
+      <c r="D88" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>350</v>
+      </c>
+      <c r="B89" t="s">
+        <v>138</v>
+      </c>
+      <c r="C89">
+        <v>31245</v>
+      </c>
+      <c r="D89" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>351</v>
+      </c>
+      <c r="B90" t="s">
+        <v>140</v>
+      </c>
+      <c r="C90">
+        <v>36589</v>
+      </c>
+      <c r="D90" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>352</v>
+      </c>
+      <c r="B91" t="s">
+        <v>142</v>
+      </c>
+      <c r="C91">
+        <v>16378</v>
+      </c>
+      <c r="D91" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>267</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>16537</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>268</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>353</v>
+      </c>
+      <c r="B92" t="s">
+        <v>143</v>
+      </c>
+      <c r="C92">
+        <v>17788</v>
+      </c>
+      <c r="D92" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>354</v>
+      </c>
+      <c r="B93" t="s">
+        <v>145</v>
+      </c>
+      <c r="C93">
+        <v>15478</v>
+      </c>
+      <c r="D93" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>355</v>
+      </c>
+      <c r="B94" t="s">
+        <v>147</v>
+      </c>
+      <c r="C94">
+        <v>37589</v>
+      </c>
+      <c r="D94" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>356</v>
+      </c>
+      <c r="B95" t="s">
+        <v>149</v>
+      </c>
+      <c r="C95">
+        <v>22255</v>
+      </c>
+      <c r="D95" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>357</v>
+      </c>
+      <c r="B96" t="s">
+        <v>151</v>
+      </c>
+      <c r="C96">
+        <v>16478</v>
+      </c>
+      <c r="D96" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>358</v>
+      </c>
+      <c r="B97" t="s">
+        <v>153</v>
+      </c>
+      <c r="C97">
+        <v>88888</v>
+      </c>
+      <c r="D97" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>359</v>
+      </c>
+      <c r="B98" t="s">
+        <v>155</v>
+      </c>
+      <c r="C98">
+        <v>66666</v>
+      </c>
+      <c r="D98" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>360</v>
+      </c>
+      <c r="B99" t="s">
+        <v>156</v>
+      </c>
+      <c r="C99">
+        <v>26478</v>
+      </c>
+      <c r="D99" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>361</v>
+      </c>
+      <c r="B100" t="s">
+        <v>157</v>
+      </c>
+      <c r="C100">
+        <v>37788</v>
+      </c>
+      <c r="D100" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>362</v>
+      </c>
+      <c r="B101" t="s">
+        <v>158</v>
+      </c>
+      <c r="C101">
         <v>15467</v>
       </c>
-      <c r="E7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>269</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8">
-        <v>71434</v>
-      </c>
-      <c r="E8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>270</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9">
-        <v>68433</v>
-      </c>
-      <c r="E9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>271</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10">
-        <v>15666</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>272</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11">
-        <v>25678</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12">
-        <v>65833</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>274</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13">
-        <v>15784</v>
-      </c>
-      <c r="E13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>275</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14">
-        <v>77456</v>
-      </c>
-      <c r="E14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>276</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15">
-        <v>25467</v>
-      </c>
-      <c r="E15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>277</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16">
-        <v>84624</v>
-      </c>
-      <c r="E16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>278</v>
-      </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17">
-        <v>99965</v>
-      </c>
-      <c r="E17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>279</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18">
-        <v>15489</v>
-      </c>
-      <c r="E18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>280</v>
-      </c>
-      <c r="C19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19">
-        <v>14354</v>
-      </c>
-      <c r="E19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>281</v>
-      </c>
-      <c r="C20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20">
-        <v>42367</v>
-      </c>
-      <c r="E20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>282</v>
-      </c>
-      <c r="C21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21">
-        <v>37689</v>
-      </c>
-      <c r="E21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>283</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22">
-        <v>25478</v>
-      </c>
-      <c r="E22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>284</v>
-      </c>
-      <c r="C23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23">
-        <v>15478</v>
-      </c>
-      <c r="E23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>285</v>
-      </c>
-      <c r="C24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24">
-        <v>73447</v>
-      </c>
-      <c r="E24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>286</v>
-      </c>
-      <c r="C25" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25">
-        <v>26589</v>
-      </c>
-      <c r="E25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>287</v>
-      </c>
-      <c r="C26" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26">
-        <v>15894</v>
-      </c>
-      <c r="E26" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>288</v>
-      </c>
-      <c r="C27" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27">
-        <v>26478</v>
-      </c>
-      <c r="E27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>289</v>
-      </c>
-      <c r="C28" t="s">
-        <v>48</v>
-      </c>
-      <c r="D28">
-        <v>55567</v>
-      </c>
-      <c r="E28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>290</v>
-      </c>
-      <c r="C29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29">
-        <v>35467</v>
-      </c>
-      <c r="E29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>291</v>
-      </c>
-      <c r="C30" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30">
-        <v>25489</v>
-      </c>
-      <c r="E30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>292</v>
-      </c>
-      <c r="C31" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31">
-        <v>12356</v>
-      </c>
-      <c r="E31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>293</v>
-      </c>
-      <c r="C32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32">
-        <v>97834</v>
-      </c>
-      <c r="E32" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>294</v>
-      </c>
-      <c r="C33" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33">
-        <v>85678</v>
-      </c>
-      <c r="E33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>295</v>
-      </c>
-      <c r="C34" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34">
-        <v>72356</v>
-      </c>
-      <c r="E34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>296</v>
-      </c>
-      <c r="C35" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35">
-        <v>68745</v>
-      </c>
-      <c r="E35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>297</v>
-      </c>
-      <c r="C36" t="s">
-        <v>59</v>
-      </c>
-      <c r="D36">
-        <v>57789</v>
-      </c>
-      <c r="E36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>298</v>
-      </c>
-      <c r="C37" t="s">
-        <v>61</v>
-      </c>
-      <c r="D37">
-        <v>46576</v>
-      </c>
-      <c r="E37" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>299</v>
-      </c>
-      <c r="C38" t="s">
-        <v>63</v>
-      </c>
-      <c r="D38">
-        <v>34598</v>
-      </c>
-      <c r="E38" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>300</v>
-      </c>
-      <c r="C39" t="s">
-        <v>65</v>
-      </c>
-      <c r="D39">
-        <v>24444</v>
-      </c>
-      <c r="E39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>301</v>
-      </c>
-      <c r="C40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40">
-        <v>15368</v>
-      </c>
-      <c r="E40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>302</v>
-      </c>
-      <c r="C41" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41">
-        <v>17689</v>
-      </c>
-      <c r="E41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>303</v>
-      </c>
-      <c r="C42" t="s">
-        <v>69</v>
-      </c>
-      <c r="D42">
-        <v>15456</v>
-      </c>
-      <c r="E42" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>304</v>
-      </c>
-      <c r="C43" t="s">
-        <v>70</v>
-      </c>
-      <c r="D43">
-        <v>16278</v>
-      </c>
-      <c r="E43" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>305</v>
-      </c>
-      <c r="C44" t="s">
-        <v>72</v>
-      </c>
-      <c r="D44">
-        <v>11111</v>
-      </c>
-      <c r="E44" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>306</v>
-      </c>
-      <c r="C45" t="s">
-        <v>73</v>
-      </c>
-      <c r="D45">
-        <v>54634</v>
-      </c>
-      <c r="E45" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46" t="s">
-        <v>307</v>
-      </c>
-      <c r="C46" t="s">
-        <v>74</v>
-      </c>
-      <c r="D46">
-        <v>15489</v>
-      </c>
-      <c r="E46" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>308</v>
-      </c>
-      <c r="C47" t="s">
-        <v>57</v>
-      </c>
-      <c r="D47">
-        <v>67677</v>
-      </c>
-      <c r="E47" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>309</v>
-      </c>
-      <c r="C48" t="s">
-        <v>75</v>
-      </c>
-      <c r="D48">
-        <v>24356</v>
-      </c>
-      <c r="E48" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49" t="s">
-        <v>310</v>
-      </c>
-      <c r="C49" t="s">
-        <v>76</v>
-      </c>
-      <c r="D49">
-        <v>36567</v>
-      </c>
-      <c r="E49" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>311</v>
-      </c>
-      <c r="C50" t="s">
-        <v>77</v>
-      </c>
-      <c r="D50">
-        <v>79834</v>
-      </c>
-      <c r="E50" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="B51" t="s">
-        <v>312</v>
-      </c>
-      <c r="C51" t="s">
-        <v>79</v>
-      </c>
-      <c r="D51">
-        <v>26567</v>
-      </c>
-      <c r="E51" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>313</v>
-      </c>
-      <c r="C52" t="s">
-        <v>80</v>
-      </c>
-      <c r="D52">
-        <v>14356</v>
-      </c>
-      <c r="E52" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="B53" t="s">
-        <v>314</v>
-      </c>
-      <c r="C53" t="s">
-        <v>81</v>
-      </c>
-      <c r="D53">
-        <v>15378</v>
-      </c>
-      <c r="E53" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="B54" t="s">
-        <v>315</v>
-      </c>
-      <c r="C54" t="s">
-        <v>83</v>
-      </c>
-      <c r="D54">
-        <v>25567</v>
-      </c>
-      <c r="E54" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="B55" t="s">
-        <v>316</v>
-      </c>
-      <c r="C55" t="s">
-        <v>85</v>
-      </c>
-      <c r="D55">
-        <v>38699</v>
-      </c>
-      <c r="E55" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56" t="s">
-        <v>317</v>
-      </c>
-      <c r="C56" t="s">
-        <v>86</v>
-      </c>
-      <c r="D56">
-        <v>44444</v>
-      </c>
-      <c r="E56" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="B57" t="s">
-        <v>318</v>
-      </c>
-      <c r="C57" t="s">
-        <v>88</v>
-      </c>
-      <c r="D57">
-        <v>52468</v>
-      </c>
-      <c r="E57" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="B58" t="s">
-        <v>319</v>
-      </c>
-      <c r="C58" t="s">
-        <v>90</v>
-      </c>
-      <c r="D58">
-        <v>61789</v>
-      </c>
-      <c r="E58" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="B59" t="s">
-        <v>320</v>
-      </c>
-      <c r="C59" t="s">
-        <v>92</v>
-      </c>
-      <c r="D59">
-        <v>71508</v>
-      </c>
-      <c r="E59" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="B60" t="s">
-        <v>321</v>
-      </c>
-      <c r="C60" t="s">
-        <v>94</v>
-      </c>
-      <c r="D60">
-        <v>82154</v>
-      </c>
-      <c r="E60" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61" t="s">
-        <v>322</v>
-      </c>
-      <c r="C61" t="s">
-        <v>96</v>
-      </c>
-      <c r="D61">
-        <v>96734</v>
-      </c>
-      <c r="E61" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="B62" t="s">
-        <v>323</v>
-      </c>
-      <c r="C62" t="s">
-        <v>98</v>
-      </c>
-      <c r="D62">
-        <v>13254</v>
-      </c>
-      <c r="E62" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="B63" t="s">
-        <v>324</v>
-      </c>
-      <c r="C63" t="s">
-        <v>99</v>
-      </c>
-      <c r="D63">
-        <v>17690</v>
-      </c>
-      <c r="E63" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64">
-        <v>63</v>
-      </c>
-      <c r="B64" t="s">
-        <v>325</v>
-      </c>
-      <c r="C64" t="s">
-        <v>101</v>
-      </c>
-      <c r="D64">
-        <v>37589</v>
-      </c>
-      <c r="E64" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65">
-        <v>64</v>
-      </c>
-      <c r="B65" t="s">
-        <v>326</v>
-      </c>
-      <c r="C65" t="s">
-        <v>103</v>
-      </c>
-      <c r="D65">
-        <v>62587</v>
-      </c>
-      <c r="E65" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66">
-        <v>65</v>
-      </c>
-      <c r="B66" t="s">
-        <v>327</v>
-      </c>
-      <c r="C66" t="s">
-        <v>105</v>
-      </c>
-      <c r="D66">
-        <v>58696</v>
-      </c>
-      <c r="E66" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <v>66</v>
-      </c>
-      <c r="B67" t="s">
-        <v>328</v>
-      </c>
-      <c r="C67" t="s">
-        <v>107</v>
-      </c>
-      <c r="D67">
-        <v>16470</v>
-      </c>
-      <c r="E67" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68">
-        <v>67</v>
-      </c>
-      <c r="B68" t="s">
-        <v>329</v>
-      </c>
-      <c r="C68" t="s">
-        <v>109</v>
-      </c>
-      <c r="D68">
-        <v>15367</v>
-      </c>
-      <c r="E68" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69">
-        <v>68</v>
-      </c>
-      <c r="B69" t="s">
-        <v>330</v>
-      </c>
-      <c r="C69" t="s">
-        <v>111</v>
-      </c>
-      <c r="D69">
-        <v>72656</v>
-      </c>
-      <c r="E69" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70">
-        <v>69</v>
-      </c>
-      <c r="B70" t="s">
-        <v>331</v>
-      </c>
-      <c r="C70" t="s">
-        <v>112</v>
-      </c>
-      <c r="D70">
-        <v>28567</v>
-      </c>
-      <c r="E70" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71">
-        <v>70</v>
-      </c>
-      <c r="B71" t="s">
-        <v>332</v>
-      </c>
-      <c r="C71" t="s">
-        <v>114</v>
-      </c>
-      <c r="D71">
-        <v>85645</v>
-      </c>
-      <c r="E71" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72">
-        <v>71</v>
-      </c>
-      <c r="B72" t="s">
-        <v>333</v>
-      </c>
-      <c r="C72" t="s">
-        <v>116</v>
-      </c>
-      <c r="D72">
-        <v>12134</v>
-      </c>
-      <c r="E72" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73">
-        <v>72</v>
-      </c>
-      <c r="B73" t="s">
-        <v>334</v>
-      </c>
-      <c r="C73" t="s">
-        <v>117</v>
-      </c>
-      <c r="D73">
-        <v>18467</v>
-      </c>
-      <c r="E73" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74">
-        <v>73</v>
-      </c>
-      <c r="B74" t="s">
-        <v>335</v>
-      </c>
-      <c r="C74" t="s">
-        <v>119</v>
-      </c>
-      <c r="D74">
-        <v>36478</v>
-      </c>
-      <c r="E74" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75">
-        <v>74</v>
-      </c>
-      <c r="B75" t="s">
-        <v>336</v>
-      </c>
-      <c r="C75" t="s">
-        <v>120</v>
-      </c>
-      <c r="D75">
-        <v>37788</v>
-      </c>
-      <c r="E75" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76">
-        <v>75</v>
-      </c>
-      <c r="B76" t="s">
-        <v>337</v>
-      </c>
-      <c r="C76" t="s">
-        <v>121</v>
-      </c>
-      <c r="D76">
-        <v>31456</v>
-      </c>
-      <c r="E76" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77">
-        <v>76</v>
-      </c>
-      <c r="B77" t="s">
-        <v>338</v>
-      </c>
-      <c r="C77" t="s">
-        <v>123</v>
-      </c>
-      <c r="D77">
-        <v>42356</v>
-      </c>
-      <c r="E77" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="B78" t="s">
-        <v>339</v>
-      </c>
-      <c r="C78" t="s">
-        <v>125</v>
-      </c>
-      <c r="D78">
-        <v>62599</v>
-      </c>
-      <c r="E78" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79">
-        <v>78</v>
-      </c>
-      <c r="B79" t="s">
-        <v>340</v>
-      </c>
-      <c r="C79" t="s">
-        <v>127</v>
-      </c>
-      <c r="D79">
-        <v>25467</v>
-      </c>
-      <c r="E79" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80">
-        <v>79</v>
-      </c>
-      <c r="B80" t="s">
-        <v>341</v>
-      </c>
-      <c r="C80" t="s">
-        <v>128</v>
-      </c>
-      <c r="D80">
-        <v>48755</v>
-      </c>
-      <c r="E80" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81">
-        <v>80</v>
-      </c>
-      <c r="B81" t="s">
-        <v>342</v>
-      </c>
-      <c r="C81" t="s">
-        <v>130</v>
-      </c>
-      <c r="D81">
-        <v>26478</v>
-      </c>
-      <c r="E81" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82">
-        <v>81</v>
-      </c>
-      <c r="B82" t="s">
-        <v>343</v>
-      </c>
-      <c r="C82" t="s">
-        <v>130</v>
-      </c>
-      <c r="D82">
-        <v>26444</v>
-      </c>
-      <c r="E82" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83">
-        <v>82</v>
-      </c>
-      <c r="B83" t="s">
-        <v>344</v>
-      </c>
-      <c r="C83" t="s">
-        <v>131</v>
-      </c>
-      <c r="D83">
-        <v>27599</v>
-      </c>
-      <c r="E83" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84">
-        <v>83</v>
-      </c>
-      <c r="B84" t="s">
-        <v>345</v>
-      </c>
-      <c r="C84" t="s">
-        <v>132</v>
-      </c>
-      <c r="D84">
-        <v>26476</v>
-      </c>
-      <c r="E84" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85">
-        <v>84</v>
-      </c>
-      <c r="B85" t="s">
-        <v>346</v>
-      </c>
-      <c r="C85" t="s">
-        <v>133</v>
-      </c>
-      <c r="D85">
-        <v>11122</v>
-      </c>
-      <c r="E85" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A86">
-        <v>85</v>
-      </c>
-      <c r="B86" t="s">
-        <v>347</v>
-      </c>
-      <c r="C86" t="s">
-        <v>134</v>
-      </c>
-      <c r="D86">
-        <v>16688</v>
-      </c>
-      <c r="E86" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87">
-        <v>86</v>
-      </c>
-      <c r="B87" t="s">
-        <v>348</v>
-      </c>
-      <c r="C87" t="s">
-        <v>135</v>
-      </c>
-      <c r="D87">
-        <v>54678</v>
-      </c>
-      <c r="E87" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88">
-        <v>87</v>
-      </c>
-      <c r="B88" t="s">
-        <v>349</v>
-      </c>
-      <c r="C88" t="s">
-        <v>136</v>
-      </c>
-      <c r="D88">
-        <v>55588</v>
-      </c>
-      <c r="E88" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A89">
-        <v>88</v>
-      </c>
-      <c r="B89" t="s">
-        <v>350</v>
-      </c>
-      <c r="C89" t="s">
-        <v>138</v>
-      </c>
-      <c r="D89">
-        <v>31245</v>
-      </c>
-      <c r="E89" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90">
-        <v>89</v>
-      </c>
-      <c r="B90" t="s">
-        <v>351</v>
-      </c>
-      <c r="C90" t="s">
-        <v>140</v>
-      </c>
-      <c r="D90">
-        <v>36589</v>
-      </c>
-      <c r="E90" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A91">
-        <v>90</v>
-      </c>
-      <c r="B91" t="s">
-        <v>352</v>
-      </c>
-      <c r="C91" t="s">
-        <v>142</v>
-      </c>
-      <c r="D91">
-        <v>16378</v>
-      </c>
-      <c r="E91" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A92">
-        <v>91</v>
-      </c>
-      <c r="B92" t="s">
-        <v>353</v>
-      </c>
-      <c r="C92" t="s">
-        <v>143</v>
-      </c>
-      <c r="D92">
-        <v>17788</v>
-      </c>
-      <c r="E92" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A93">
-        <v>92</v>
-      </c>
-      <c r="B93" t="s">
-        <v>354</v>
-      </c>
-      <c r="C93" t="s">
-        <v>145</v>
-      </c>
-      <c r="D93">
-        <v>15478</v>
-      </c>
-      <c r="E93" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A94">
-        <v>93</v>
-      </c>
-      <c r="B94" t="s">
-        <v>355</v>
-      </c>
-      <c r="C94" t="s">
-        <v>147</v>
-      </c>
-      <c r="D94">
-        <v>37589</v>
-      </c>
-      <c r="E94" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A95">
-        <v>94</v>
-      </c>
-      <c r="B95" t="s">
-        <v>356</v>
-      </c>
-      <c r="C95" t="s">
-        <v>149</v>
-      </c>
-      <c r="D95">
-        <v>22255</v>
-      </c>
-      <c r="E95" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A96">
-        <v>95</v>
-      </c>
-      <c r="B96" t="s">
-        <v>357</v>
-      </c>
-      <c r="C96" t="s">
-        <v>151</v>
-      </c>
-      <c r="D96">
-        <v>16478</v>
-      </c>
-      <c r="E96" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A97">
-        <v>96</v>
-      </c>
-      <c r="B97" t="s">
-        <v>358</v>
-      </c>
-      <c r="C97" t="s">
-        <v>153</v>
-      </c>
-      <c r="D97">
-        <v>88888</v>
-      </c>
-      <c r="E97" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A98">
-        <v>97</v>
-      </c>
-      <c r="B98" t="s">
-        <v>359</v>
-      </c>
-      <c r="C98" t="s">
-        <v>155</v>
-      </c>
-      <c r="D98">
-        <v>66666</v>
-      </c>
-      <c r="E98" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A99">
-        <v>98</v>
-      </c>
-      <c r="B99" t="s">
-        <v>360</v>
-      </c>
-      <c r="C99" t="s">
-        <v>156</v>
-      </c>
-      <c r="D99">
-        <v>26478</v>
-      </c>
-      <c r="E99" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A100">
-        <v>99</v>
-      </c>
-      <c r="B100" t="s">
-        <v>361</v>
-      </c>
-      <c r="C100" t="s">
-        <v>157</v>
-      </c>
-      <c r="D100">
-        <v>37788</v>
-      </c>
-      <c r="E100" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A101">
-        <v>100</v>
-      </c>
-      <c r="B101" t="s">
-        <v>362</v>
-      </c>
-      <c r="C101" t="s">
-        <v>158</v>
-      </c>
-      <c r="D101">
-        <v>15467</v>
-      </c>
-      <c r="E101" t="s">
+      <c r="D101" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3191,8 +2888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.3828125" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -4074,24 +3771,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAFD4BDE-D7FC-4B16-9327-C2010CA5DEB3}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.3828125" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>366</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>